<commit_message>
feat: Add yearly analysis and comprehensive statistics reporting
- Add extract_yearly_analysis.py for yearly question/division/department scoring
- Add diagnose_data_discrepancy.py to analyze data cleaning steps
- Add check_missing_scores.py to verify missing score counts
- Add generate_statistics_report.py for comprehensive statistics report
- Generate detailed Excel reports with sample counts and exclusion breakdowns
- Identify and document data quality issues (647 samples excluded in 2022)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/rawdata/부서_부문_매핑.xlsx
+++ b/rawdata/부서_부문_매핑.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\작업폴더\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$439</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$440</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="451">
   <si>
     <t>부문</t>
   </si>
@@ -1385,6 +1385,10 @@
   </si>
   <si>
     <t>간호부문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>62 Unit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1756,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C439"/>
+  <dimension ref="A1:C440"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="W135" sqref="W135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4010,9 +4014,11 @@
         <v>449</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C221" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
@@ -4021,9 +4027,7 @@
       <c r="B222" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C222" s="1" t="s">
-        <v>404</v>
-      </c>
+      <c r="C222" s="1"/>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
@@ -4033,7 +4037,7 @@
         <v>16</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>30</v>
+        <v>404</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
@@ -4044,7 +4048,7 @@
         <v>16</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>367</v>
+        <v>30</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
@@ -4055,7 +4059,7 @@
         <v>16</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>163</v>
+        <v>367</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
@@ -4066,7 +4070,7 @@
         <v>16</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>233</v>
+        <v>163</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
@@ -4077,7 +4081,7 @@
         <v>16</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>37</v>
+        <v>233</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
@@ -4088,7 +4092,7 @@
         <v>16</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>249</v>
+        <v>37</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
@@ -4099,7 +4103,7 @@
         <v>16</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>48</v>
+        <v>249</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
@@ -4110,7 +4114,7 @@
         <v>16</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>257</v>
+        <v>48</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
@@ -4121,7 +4125,7 @@
         <v>16</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
@@ -4129,9 +4133,11 @@
         <v>449</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C232" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
@@ -4140,9 +4146,7 @@
       <c r="B233" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C233" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="C233" s="1"/>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
@@ -4152,7 +4156,7 @@
         <v>8</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
@@ -4163,7 +4167,7 @@
         <v>8</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
@@ -4174,7 +4178,7 @@
         <v>8</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
@@ -4185,7 +4189,7 @@
         <v>8</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
@@ -4196,7 +4200,7 @@
         <v>8</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>260</v>
+        <v>55</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
@@ -4207,7 +4211,7 @@
         <v>8</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
@@ -4218,7 +4222,7 @@
         <v>8</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>309</v>
+        <v>259</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
@@ -4229,7 +4233,7 @@
         <v>8</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>34</v>
+        <v>309</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
@@ -4240,7 +4244,7 @@
         <v>8</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>111</v>
+        <v>34</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
@@ -4251,7 +4255,7 @@
         <v>8</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
@@ -4259,9 +4263,11 @@
         <v>449</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C244" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
@@ -4270,9 +4276,7 @@
       <c r="B245" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C245" s="1" t="s">
-        <v>197</v>
-      </c>
+      <c r="C245" s="1"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
@@ -4282,7 +4286,7 @@
         <v>72</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
@@ -4293,7 +4297,7 @@
         <v>72</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>127</v>
+        <v>238</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
@@ -4304,7 +4308,7 @@
         <v>72</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
@@ -4315,7 +4319,7 @@
         <v>72</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
@@ -4326,7 +4330,7 @@
         <v>72</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>247</v>
+        <v>116</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
@@ -4337,7 +4341,7 @@
         <v>72</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>293</v>
+        <v>247</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
@@ -4348,7 +4352,7 @@
         <v>72</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>334</v>
+        <v>293</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
@@ -4359,7 +4363,7 @@
         <v>72</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>226</v>
+        <v>334</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
@@ -4367,9 +4371,11 @@
         <v>449</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C254" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
@@ -4378,9 +4384,7 @@
       <c r="B255" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C255" s="1" t="s">
-        <v>191</v>
-      </c>
+      <c r="C255" s="1"/>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
@@ -4390,7 +4394,7 @@
         <v>57</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
@@ -4401,7 +4405,7 @@
         <v>57</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
@@ -4412,7 +4416,7 @@
         <v>57</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>193</v>
+        <v>262</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
@@ -4423,7 +4427,7 @@
         <v>57</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>301</v>
+        <v>193</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
@@ -4434,7 +4438,7 @@
         <v>57</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
@@ -4445,7 +4449,7 @@
         <v>57</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>58</v>
+        <v>292</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
@@ -4456,7 +4460,7 @@
         <v>57</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>187</v>
+        <v>58</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
@@ -4467,7 +4471,7 @@
         <v>57</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>265</v>
+        <v>187</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
@@ -4478,7 +4482,7 @@
         <v>57</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>361</v>
+        <v>265</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
@@ -4489,7 +4493,7 @@
         <v>57</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>121</v>
+        <v>361</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
@@ -4497,9 +4501,11 @@
         <v>449</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C266" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
@@ -4508,9 +4514,7 @@
       <c r="B267" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C267" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="C267" s="1"/>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
@@ -4520,7 +4524,7 @@
         <v>20</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>69</v>
+        <v>161</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
@@ -4531,7 +4535,7 @@
         <v>20</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>234</v>
+        <v>69</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
@@ -4542,7 +4546,7 @@
         <v>20</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
@@ -4553,7 +4557,7 @@
         <v>20</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
@@ -4564,7 +4568,7 @@
         <v>20</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>241</v>
+        <v>130</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
@@ -4575,7 +4579,7 @@
         <v>20</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>133</v>
+        <v>241</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
@@ -4586,7 +4590,7 @@
         <v>20</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
@@ -4594,9 +4598,11 @@
         <v>449</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C275" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
@@ -4605,9 +4611,7 @@
       <c r="B276" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C276" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="C276" s="1"/>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
@@ -4617,7 +4621,7 @@
         <v>76</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>320</v>
+        <v>138</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
@@ -4628,7 +4632,7 @@
         <v>76</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>115</v>
+        <v>320</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
@@ -4639,7 +4643,7 @@
         <v>76</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
@@ -4650,7 +4654,7 @@
         <v>76</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>214</v>
+        <v>77</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
@@ -4661,7 +4665,7 @@
         <v>76</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
@@ -4669,9 +4673,11 @@
         <v>449</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C282" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
@@ -4680,9 +4686,7 @@
       <c r="B283" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C283" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="C283" s="1"/>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
@@ -4692,7 +4696,7 @@
         <v>12</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
@@ -4703,7 +4707,7 @@
         <v>12</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>217</v>
+        <v>13</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
@@ -4714,7 +4718,7 @@
         <v>12</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>183</v>
+        <v>217</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
@@ -4725,7 +4729,7 @@
         <v>12</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>101</v>
+        <v>183</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
@@ -4736,7 +4740,7 @@
         <v>12</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
@@ -4747,7 +4751,7 @@
         <v>12</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>215</v>
+        <v>31</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
@@ -4758,24 +4762,26 @@
         <v>12</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>63</v>
+        <v>215</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C291" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>444</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="C292" s="1"/>
     </row>
@@ -4786,18 +4792,18 @@
       <c r="B293" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C293" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="C293" s="1"/>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>444</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C294" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
@@ -4806,18 +4812,18 @@
       <c r="B295" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C295" s="1" t="s">
-        <v>270</v>
-      </c>
+      <c r="C295" s="1"/>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>444</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C296" s="1"/>
+        <v>269</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
@@ -4826,9 +4832,7 @@
       <c r="B297" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C297" s="1" t="s">
-        <v>368</v>
-      </c>
+      <c r="C297" s="1"/>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
@@ -4838,24 +4842,26 @@
         <v>271</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>302</v>
+        <v>368</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C299" s="1"/>
+        <v>271</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
         <v>443</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>394</v>
+        <v>434</v>
       </c>
       <c r="C300" s="1"/>
     </row>
@@ -4866,25 +4872,25 @@
       <c r="B301" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="C301" s="1" t="s">
-        <v>395</v>
-      </c>
+      <c r="C301" s="1"/>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
         <v>443</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C302" s="1"/>
+        <v>394</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
         <v>443</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>390</v>
+        <v>411</v>
       </c>
       <c r="C303" s="1"/>
     </row>
@@ -4893,7 +4899,7 @@
         <v>443</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="C304" s="1"/>
     </row>
@@ -4902,7 +4908,7 @@
         <v>443</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C305" s="1"/>
     </row>
@@ -4911,7 +4917,7 @@
         <v>443</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>346</v>
+        <v>175</v>
       </c>
       <c r="C306" s="1"/>
     </row>
@@ -4922,9 +4928,7 @@
       <c r="B307" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C307" s="1" t="s">
-        <v>347</v>
-      </c>
+      <c r="C307" s="1"/>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
@@ -4934,7 +4938,7 @@
         <v>346</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>392</v>
+        <v>347</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
@@ -4942,16 +4946,18 @@
         <v>443</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C309" s="1"/>
+        <v>346</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" s="1" t="s">
         <v>443</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>199</v>
+        <v>19</v>
       </c>
       <c r="C310" s="1"/>
     </row>
@@ -4962,25 +4968,25 @@
       <c r="B311" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C311" s="1" t="s">
-        <v>200</v>
-      </c>
+      <c r="C311" s="1"/>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
         <v>443</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C312" s="1"/>
+        <v>199</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
         <v>443</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>275</v>
+        <v>305</v>
       </c>
       <c r="C313" s="1"/>
     </row>
@@ -4989,7 +4995,7 @@
         <v>443</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="C314" s="1"/>
     </row>
@@ -4998,7 +5004,7 @@
         <v>443</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>29</v>
+        <v>294</v>
       </c>
       <c r="C315" s="1"/>
     </row>
@@ -5007,7 +5013,7 @@
         <v>443</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="C316" s="1"/>
     </row>
@@ -5018,9 +5024,7 @@
       <c r="B317" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C317" s="1" t="s">
-        <v>280</v>
-      </c>
+      <c r="C317" s="1"/>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
@@ -5030,7 +5034,7 @@
         <v>88</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>89</v>
+        <v>280</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
@@ -5041,7 +5045,7 @@
         <v>88</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>220</v>
+        <v>89</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
@@ -5052,7 +5056,7 @@
         <v>88</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>289</v>
+        <v>220</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
@@ -5063,7 +5067,7 @@
         <v>88</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>94</v>
+        <v>289</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
@@ -5074,7 +5078,7 @@
         <v>88</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>328</v>
+        <v>94</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
@@ -5082,10 +5086,10 @@
         <v>443</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>204</v>
+        <v>88</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.3">
@@ -5096,7 +5100,7 @@
         <v>204</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>205</v>
+        <v>350</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
@@ -5104,16 +5108,18 @@
         <v>443</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C325" s="1"/>
+        <v>204</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
         <v>443</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>419</v>
+        <v>402</v>
       </c>
       <c r="C326" s="1"/>
     </row>
@@ -5122,16 +5128,16 @@
         <v>443</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>277</v>
+        <v>419</v>
       </c>
       <c r="C327" s="1"/>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>396</v>
+        <v>277</v>
       </c>
       <c r="C328" s="1"/>
     </row>
@@ -5142,18 +5148,18 @@
       <c r="B329" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C329" s="1" t="s">
-        <v>408</v>
-      </c>
+      <c r="C329" s="1"/>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
         <v>442</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C330" s="1"/>
+        <v>396</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
@@ -5162,9 +5168,7 @@
       <c r="B331" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C331" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="C331" s="1"/>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
@@ -5174,7 +5178,7 @@
         <v>118</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>383</v>
+        <v>119</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
@@ -5185,7 +5189,7 @@
         <v>118</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>335</v>
+        <v>383</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
@@ -5196,7 +5200,7 @@
         <v>118</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>387</v>
+        <v>335</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
@@ -5207,7 +5211,7 @@
         <v>118</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>417</v>
+        <v>387</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
@@ -5215,9 +5219,11 @@
         <v>442</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C336" s="1"/>
+        <v>118</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" s="1" t="s">
@@ -5226,18 +5232,18 @@
       <c r="B337" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C337" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="C337" s="1"/>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C338" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
@@ -5246,9 +5252,7 @@
       <c r="B339" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C339" s="1" t="s">
-        <v>351</v>
-      </c>
+      <c r="C339" s="1"/>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" s="1" t="s">
@@ -5258,7 +5262,7 @@
         <v>323</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>324</v>
+        <v>351</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
@@ -5269,24 +5273,26 @@
         <v>323</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>410</v>
+        <v>324</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C342" s="1"/>
+        <v>323</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" s="1" t="s">
         <v>440</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>152</v>
+        <v>90</v>
       </c>
       <c r="C343" s="1"/>
     </row>
@@ -5297,9 +5303,7 @@
       <c r="B344" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C344" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="C344" s="1"/>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
@@ -5309,7 +5313,7 @@
         <v>152</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>208</v>
+        <v>153</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
@@ -5317,9 +5321,11 @@
         <v>440</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C346" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A347" s="1" t="s">
@@ -5328,9 +5334,7 @@
       <c r="B347" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C347" s="1" t="s">
-        <v>378</v>
-      </c>
+      <c r="C347" s="1"/>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
@@ -5340,7 +5344,7 @@
         <v>244</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
@@ -5348,9 +5352,11 @@
         <v>440</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C349" s="1"/>
+        <v>244</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350" s="1" t="s">
@@ -5359,9 +5365,7 @@
       <c r="B350" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="C350" s="1" t="s">
-        <v>415</v>
-      </c>
+      <c r="C350" s="1"/>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
@@ -5371,17 +5375,19 @@
         <v>344</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>345</v>
+        <v>415</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C352" s="1"/>
+        <v>344</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
@@ -5390,9 +5396,7 @@
       <c r="B353" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C353" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="C353" s="1"/>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A354" s="1" t="s">
@@ -5402,7 +5406,7 @@
         <v>50</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>376</v>
+        <v>51</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.3">
@@ -5410,16 +5414,18 @@
         <v>439</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="C355" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A356" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>212</v>
+        <v>426</v>
       </c>
       <c r="C356" s="1"/>
     </row>
@@ -5430,9 +5436,7 @@
       <c r="B357" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C357" s="1" t="s">
-        <v>386</v>
-      </c>
+      <c r="C357" s="1"/>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A358" s="1" t="s">
@@ -5442,7 +5446,7 @@
         <v>212</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>295</v>
+        <v>386</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.3">
@@ -5453,7 +5457,7 @@
         <v>212</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>213</v>
+        <v>295</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.3">
@@ -5461,9 +5465,11 @@
         <v>438</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C360" s="1"/>
+        <v>212</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
@@ -5472,9 +5478,7 @@
       <c r="B361" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C361" s="1" t="s">
-        <v>288</v>
-      </c>
+      <c r="C361" s="1"/>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A362" s="1" t="s">
@@ -5484,7 +5488,7 @@
         <v>287</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>391</v>
+        <v>288</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.3">
@@ -5492,9 +5496,11 @@
         <v>438</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C363" s="1"/>
+        <v>287</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
@@ -5503,9 +5509,7 @@
       <c r="B364" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C364" s="1" t="s">
-        <v>401</v>
-      </c>
+      <c r="C364" s="1"/>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A365" s="1" t="s">
@@ -5515,7 +5519,7 @@
         <v>358</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>359</v>
+        <v>401</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.3">
@@ -5523,9 +5527,11 @@
         <v>438</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C366" s="1"/>
+        <v>358</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A367" s="1" t="s">
@@ -5534,9 +5540,7 @@
       <c r="B367" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C367" s="1" t="s">
-        <v>149</v>
-      </c>
+      <c r="C367" s="1"/>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
@@ -5546,7 +5550,7 @@
         <v>148</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>245</v>
+        <v>149</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
@@ -5557,17 +5561,19 @@
         <v>148</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>176</v>
+        <v>245</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C370" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
@@ -5576,9 +5582,7 @@
       <c r="B371" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C371" s="1" t="s">
-        <v>284</v>
-      </c>
+      <c r="C371" s="1"/>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
@@ -5588,7 +5592,7 @@
         <v>210</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>224</v>
+        <v>284</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
@@ -5599,7 +5603,7 @@
         <v>210</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
@@ -5607,9 +5611,11 @@
         <v>437</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C374" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A375" s="1" t="s">
@@ -5618,18 +5624,18 @@
       <c r="B375" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C375" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="C375" s="1"/>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A376" s="1" t="s">
         <v>437</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C376" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A377" s="1" t="s">
@@ -5638,9 +5644,7 @@
       <c r="B377" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="C377" s="1" t="s">
-        <v>406</v>
-      </c>
+      <c r="C377" s="1"/>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A378" s="1" t="s">
@@ -5650,7 +5654,7 @@
         <v>352</v>
       </c>
       <c r="C378" s="1" t="s">
-        <v>373</v>
+        <v>406</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
@@ -5658,9 +5662,11 @@
         <v>437</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C379" s="1"/>
+        <v>352</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
@@ -5669,9 +5675,7 @@
       <c r="B380" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C380" s="1" t="s">
-        <v>227</v>
-      </c>
+      <c r="C380" s="1"/>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A381" s="1" t="s">
@@ -5681,7 +5685,7 @@
         <v>84</v>
       </c>
       <c r="C381" s="1" t="s">
-        <v>303</v>
+        <v>227</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
@@ -5692,7 +5696,7 @@
         <v>84</v>
       </c>
       <c r="C382" s="1" t="s">
-        <v>203</v>
+        <v>303</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
@@ -5700,9 +5704,11 @@
         <v>437</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C383" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="C383" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
@@ -5711,9 +5717,7 @@
       <c r="B384" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C384" s="1" t="s">
-        <v>399</v>
-      </c>
+      <c r="C384" s="1"/>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
@@ -5723,7 +5727,7 @@
         <v>44</v>
       </c>
       <c r="C385" s="1" t="s">
-        <v>45</v>
+        <v>399</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.3">
@@ -5731,9 +5735,11 @@
         <v>437</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C386" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
@@ -5742,9 +5748,7 @@
       <c r="B387" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C387" s="1" t="s">
-        <v>420</v>
-      </c>
+      <c r="C387" s="1"/>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
@@ -5754,7 +5758,7 @@
         <v>46</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>339</v>
+        <v>420</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.3">
@@ -5765,7 +5769,7 @@
         <v>46</v>
       </c>
       <c r="C389" s="1" t="s">
-        <v>253</v>
+        <v>339</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.3">
@@ -5776,7 +5780,7 @@
         <v>46</v>
       </c>
       <c r="C390" s="1" t="s">
-        <v>370</v>
+        <v>253</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
@@ -5784,9 +5788,11 @@
         <v>437</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C391" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
@@ -5795,9 +5801,7 @@
       <c r="B392" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C392" s="1" t="s">
-        <v>407</v>
-      </c>
+      <c r="C392" s="1"/>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
@@ -5807,7 +5811,7 @@
         <v>336</v>
       </c>
       <c r="C393" s="1" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.3">
@@ -5818,7 +5822,7 @@
         <v>336</v>
       </c>
       <c r="C394" s="1" t="s">
-        <v>337</v>
+        <v>398</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.3">
@@ -5826,9 +5830,11 @@
         <v>437</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C395" s="1"/>
+        <v>336</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
@@ -5837,9 +5843,7 @@
       <c r="B396" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C396" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="C396" s="1"/>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
@@ -5849,7 +5853,7 @@
         <v>23</v>
       </c>
       <c r="C397" s="1" t="s">
-        <v>315</v>
+        <v>24</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.3">
@@ -5860,7 +5864,7 @@
         <v>23</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>385</v>
+        <v>315</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.3">
@@ -5868,9 +5872,11 @@
         <v>437</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C399" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
@@ -5879,9 +5885,7 @@
       <c r="B400" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C400" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="C400" s="1"/>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A401" s="1" t="s">
@@ -5891,7 +5895,7 @@
         <v>98</v>
       </c>
       <c r="C401" s="1" t="s">
-        <v>369</v>
+        <v>99</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.3">
@@ -5899,9 +5903,11 @@
         <v>437</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C402" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
@@ -5910,9 +5916,7 @@
       <c r="B403" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C403" s="1" t="s">
-        <v>252</v>
-      </c>
+      <c r="C403" s="1"/>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
@@ -5922,7 +5926,7 @@
         <v>62</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>182</v>
+        <v>252</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.3">
@@ -5930,9 +5934,11 @@
         <v>437</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C405" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="C405" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
@@ -5941,9 +5947,7 @@
       <c r="B406" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C406" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="C406" s="1"/>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
@@ -5953,7 +5957,7 @@
         <v>65</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>365</v>
+        <v>100</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.3">
@@ -5964,7 +5968,7 @@
         <v>65</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>178</v>
+        <v>365</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.3">
@@ -5975,7 +5979,7 @@
         <v>65</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>67</v>
+        <v>178</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.3">
@@ -5986,7 +5990,7 @@
         <v>65</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.3">
@@ -5994,9 +5998,11 @@
         <v>437</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C411" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A412" s="1" t="s">
@@ -6005,9 +6011,7 @@
       <c r="B412" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C412" s="1" t="s">
-        <v>186</v>
-      </c>
+      <c r="C412" s="1"/>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A413" s="1" t="s">
@@ -6017,7 +6021,7 @@
         <v>82</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>83</v>
+        <v>186</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.3">
@@ -6025,9 +6029,11 @@
         <v>437</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C414" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A415" s="1" t="s">
@@ -6036,9 +6042,7 @@
       <c r="B415" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C415" s="1" t="s">
-        <v>422</v>
-      </c>
+      <c r="C415" s="1"/>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A416" s="1" t="s">
@@ -6048,7 +6052,7 @@
         <v>414</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.3">
@@ -6056,9 +6060,11 @@
         <v>437</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C417" s="1"/>
+        <v>414</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A418" s="1" t="s">
@@ -6067,9 +6073,7 @@
       <c r="B418" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C418" s="1" t="s">
-        <v>428</v>
-      </c>
+      <c r="C418" s="1"/>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A419" s="1" t="s">
@@ -6079,7 +6083,7 @@
         <v>228</v>
       </c>
       <c r="C419" s="1" t="s">
-        <v>229</v>
+        <v>428</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.3">
@@ -6087,16 +6091,18 @@
         <v>437</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="C420" s="1"/>
+        <v>228</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
         <v>437</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>201</v>
+        <v>429</v>
       </c>
       <c r="C421" s="1"/>
     </row>
@@ -6105,16 +6111,16 @@
         <v>437</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>421</v>
+        <v>201</v>
       </c>
       <c r="C422" s="1"/>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A423" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>313</v>
+        <v>421</v>
       </c>
       <c r="C423" s="1"/>
     </row>
@@ -6125,9 +6131,7 @@
       <c r="B424" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C424" s="1" t="s">
-        <v>314</v>
-      </c>
+      <c r="C424" s="1"/>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A425" s="1" t="s">
@@ -6137,7 +6141,7 @@
         <v>313</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>374</v>
+        <v>314</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.3">
@@ -6145,9 +6149,11 @@
         <v>436</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C426" s="1"/>
+        <v>313</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A427" s="1" t="s">
@@ -6156,25 +6162,25 @@
       <c r="B427" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C427" s="1" t="s">
-        <v>317</v>
-      </c>
+      <c r="C427" s="1"/>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A428" s="1" t="s">
         <v>436</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C428" s="1"/>
+        <v>316</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A429" s="1" t="s">
         <v>436</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="C429" s="1"/>
     </row>
@@ -6183,7 +6189,7 @@
         <v>436</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="C430" s="1"/>
     </row>
@@ -6194,25 +6200,25 @@
       <c r="B431" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="C431" s="1" t="s">
-        <v>380</v>
-      </c>
+      <c r="C431" s="1"/>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A432" s="1" t="s">
         <v>436</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C432" s="1"/>
+        <v>379</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A433" s="1" t="s">
         <v>436</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>160</v>
+        <v>78</v>
       </c>
       <c r="C433" s="1"/>
     </row>
@@ -6221,7 +6227,7 @@
         <v>436</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>207</v>
+        <v>160</v>
       </c>
       <c r="C434" s="1"/>
     </row>
@@ -6230,7 +6236,7 @@
         <v>436</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>432</v>
+        <v>207</v>
       </c>
       <c r="C435" s="1"/>
     </row>
@@ -6239,7 +6245,7 @@
         <v>436</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>409</v>
+        <v>432</v>
       </c>
       <c r="C436" s="1"/>
     </row>
@@ -6248,7 +6254,7 @@
         <v>436</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>184</v>
+        <v>409</v>
       </c>
       <c r="C437" s="1"/>
     </row>
@@ -6259,21 +6265,30 @@
       <c r="B438" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C438" s="1" t="s">
-        <v>413</v>
-      </c>
+      <c r="C438" s="1"/>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
         <v>436</v>
       </c>
       <c r="B439" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A440" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B440" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="C439" s="1"/>
+      <c r="C440" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C439"/>
+  <autoFilter ref="A1:C440"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>